<commit_message>
jxls-excel-upload: add date format fucntion fn
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/templates/board.xlsx
+++ b/src/main/resources/static/excel/templates/board.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\excel\src\main\resources\templates\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\excel\src\main\resources\static\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C7313-8011-43B8-9F55-09AE11F9654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1F6A02-2A7F-490A-BF04-022A0FD0E3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41670" yWindow="6645" windowWidth="21600" windowHeight="8655" xr2:uid="{EAEC43BA-4267-4B0D-85BE-8102AC982A62}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAEC43BA-4267-4B0D-85BE-8102AC982A62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,13 +120,15 @@
     <t>${item.likeIt}</t>
   </si>
   <si>
-    <t>${item.createDate}</t>
-  </si>
-  <si>
-    <t>${item.updateDate}</t>
-  </si>
-  <si>
     <t>${item.id}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(item.createDate, 'yyyy-MM-dd HH:mm:ss')}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(item.updateDate, 'yyyy-MM-dd HH:mm:ss')}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -640,7 +642,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -680,7 +682,7 @@
     </row>
     <row r="2" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -698,10 +700,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>